<commit_message>
found new level shifter. Need to put in schematic
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.3-bom.xlsx
+++ b/sedani/estop/estop-1.3-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121C87C1-34C1-4DF4-BBDD-4DCB8A0A1B5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A4E20A-8F71-4B78-BA48-C8EA7B1D8F4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Unit Cost</t>
   </si>
   <si>
-    <t>401-1426-1-ND</t>
-  </si>
-  <si>
     <t>0.1uF ceramic</t>
   </si>
   <si>
@@ -244,9 +241,6 @@
     <t>SMD LEDs</t>
   </si>
   <si>
-    <t>296-12163-1-ND</t>
-  </si>
-  <si>
     <t>USB mini header</t>
   </si>
   <si>
@@ -263,6 +257,15 @@
   </si>
   <si>
     <t>507-1797-1-ND</t>
+  </si>
+  <si>
+    <t>H2960CT-ND</t>
+  </si>
+  <si>
+    <t>1727-4290-1-ND</t>
+  </si>
+  <si>
+    <t>401-1426-1-ND (CAD from  296-1135-1-ND)</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,14 +294,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -341,9 +336,6 @@
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -632,7 +624,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,13 +647,13 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -673,13 +665,13 @@
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -691,15 +683,15 @@
         <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2">
         <v>4.12</v>
@@ -709,10 +701,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="K2" s="1">
         <v>1</v>
@@ -730,10 +722,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2">
         <v>5.95</v>
@@ -743,10 +735,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="K3" s="1">
         <v>1</v>
@@ -777,10 +769,10 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="K4" s="1">
         <v>1</v>
@@ -811,10 +803,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="K5" s="1">
         <v>1</v>
@@ -832,7 +824,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -845,10 +837,10 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K6" s="1">
         <v>1</v>
@@ -869,7 +861,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="2">
         <v>0.15</v>
@@ -879,10 +871,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K7" s="1">
         <v>1</v>
@@ -900,10 +892,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="2">
         <v>3.4000000000000002E-2</v>
@@ -913,10 +905,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K8" s="1">
         <v>1</v>
@@ -934,10 +926,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="2">
         <v>3.3000000000000002E-2</v>
@@ -947,10 +939,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9" s="1">
         <v>1</v>
@@ -968,10 +960,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2">
         <v>1.9E-2</v>
@@ -981,7 +973,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K10" s="1">
         <v>2</v>
@@ -996,10 +988,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="2">
         <v>2.1999999999999999E-2</v>
@@ -1009,10 +1001,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="K11" s="1">
         <v>1</v>
@@ -1030,10 +1022,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3"/>
       <c r="F12" s="2">
@@ -1044,10 +1036,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K12" s="1">
         <v>1</v>
@@ -1068,7 +1060,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="2">
         <v>1.4999999999999999E-2</v>
@@ -1078,10 +1070,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="K13" s="1">
         <v>1</v>
@@ -1102,7 +1094,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="F14" s="2">
         <v>0.52</v>
@@ -1112,10 +1104,10 @@
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K14" s="1">
         <v>1</v>
@@ -1131,23 +1123,25 @@
         <v>2.95</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="D15" s="6"/>
       <c r="I15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K15" s="1">
         <v>1</v>
@@ -1163,18 +1157,18 @@
         <v>1.25</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K16" s="1">
         <v>1</v>
@@ -1192,10 +1186,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" s="2">
         <v>2.17</v>
@@ -1207,7 +1201,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
       </c>
       <c r="N18" s="2">
         <f>SUM(N2:N16)</f>
@@ -1216,10 +1216,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
         <v>74</v>
-      </c>
-      <c r="B19" t="s">
-        <v>76</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1230,10 +1230,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -1250,15 +1250,15 @@
     </row>
     <row r="29" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="F30" s="2">
         <v>7.66</v>

</xml_diff>

<commit_message>
schematic fixed with new level shifter
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.3-bom.xlsx
+++ b/sedani/estop/estop-1.3-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A4E20A-8F71-4B78-BA48-C8EA7B1D8F4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DA48A9-334F-4003-92A5-97B8CEB21410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="86">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -262,10 +262,28 @@
     <t>H2960CT-ND</t>
   </si>
   <si>
-    <t>1727-4290-1-ND</t>
-  </si>
-  <si>
     <t>401-1426-1-ND (CAD from  296-1135-1-ND)</t>
+  </si>
+  <si>
+    <t>Mux</t>
+  </si>
+  <si>
+    <t>External Watchdog</t>
+  </si>
+  <si>
+    <t>SR latch</t>
+  </si>
+  <si>
+    <t>296-31498-1-ND</t>
+  </si>
+  <si>
+    <t>MC74HC157ADGOS-ND</t>
+  </si>
+  <si>
+    <t>296-1135-1-ND</t>
+  </si>
+  <si>
+    <t>APX823-31W5GDICT-ND</t>
   </si>
 </sst>
 </file>
@@ -320,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -340,6 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -621,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,7 +1113,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F14" s="2">
         <v>0.52</v>
@@ -1131,10 +1150,10 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C15" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D15" s="6"/>
       <c r="I15" s="1" t="s">
@@ -1242,15 +1261,15 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G28" s="2">
-        <f>SUM(G2:G27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="24" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G25" s="2">
+        <f>SUM(G2:G24)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
@@ -1260,8 +1279,29 @@
       <c r="B30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="2">
-        <v>7.66</v>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1271,8 +1311,11 @@
     <hyperlink ref="J12" r:id="rId3" xr:uid="{F8FCF166-57E3-4B3F-A665-042561BF6934}"/>
     <hyperlink ref="J15" r:id="rId4" xr:uid="{FBC8E941-7B24-4FAF-ACEB-DD0438F6BDD9}"/>
     <hyperlink ref="J16" r:id="rId5" xr:uid="{47868E09-3EC4-42BC-8E64-F5105C27F835}"/>
+    <hyperlink ref="B33" r:id="rId6" xr:uid="{5C805838-9D7A-4A69-B716-8DBFF1B315E3}"/>
+    <hyperlink ref="B32" r:id="rId7" xr:uid="{2DE54676-3B1A-4A9B-8385-E44AE31DB6F7}"/>
+    <hyperlink ref="B31" r:id="rId8" xr:uid="{8C8CAB8B-5DD6-4EB4-AD24-EE91835A4ED0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made crystal lines same size
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.3-bom.xlsx
+++ b/sedani/estop/estop-1.3-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DA48A9-334F-4003-92A5-97B8CEB21410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA624842-2841-463E-A12C-F3B36AF33899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated diode + fuse values
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.3-bom.xlsx
+++ b/sedani/estop/estop-1.3-bom.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239B58A4-B675-4E21-951F-799B40E08E5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8839E6-F61C-4A77-9A4A-C199EB0667C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -241,18 +241,9 @@
     <t>300mA Schottky diode</t>
   </si>
   <si>
-    <t>300mA fuse</t>
-  </si>
-  <si>
-    <t>NSR0530HT1GOSCT-ND</t>
-  </si>
-  <si>
     <t>Per board</t>
   </si>
   <si>
-    <t>507-1797-1-ND</t>
-  </si>
-  <si>
     <t>H2960CT-ND</t>
   </si>
   <si>
@@ -299,6 +290,15 @@
   </si>
   <si>
     <t>RF SMA PCB connector</t>
+  </si>
+  <si>
+    <t>507-1800-1-ND</t>
+  </si>
+  <si>
+    <t>350mA fuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B5819WS-TPMSCT-ND </t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,7 +690,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1052,10 +1052,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1082,10 +1082,10 @@
     </row>
     <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1229,10 +1229,10 @@
     </row>
     <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -1262,7 +1262,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -1280,7 +1280,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>18</v>
@@ -1323,7 +1323,7 @@
         <v>69</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1334,21 +1334,21 @@
         <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="F22" s="2">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -1373,26 +1373,26 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved BOM to right branch
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.3-bom.xlsx
+++ b/sedani/estop/estop-1.3-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8839E6-F61C-4A77-9A4A-C199EB0667C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D780EC-453C-45FD-9ABE-C2BC38B7E288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -232,19 +232,19 @@
     <t>1597-1488-ND</t>
   </si>
   <si>
-    <t>SMD LEDs</t>
-  </si>
-  <si>
-    <t>USB mini header</t>
-  </si>
-  <si>
     <t>300mA Schottky diode</t>
   </si>
   <si>
+    <t>300mA fuse</t>
+  </si>
+  <si>
+    <t>NSR0530HT1GOSCT-ND</t>
+  </si>
+  <si>
     <t>Per board</t>
   </si>
   <si>
-    <t>H2960CT-ND</t>
+    <t>507-1797-1-ND</t>
   </si>
   <si>
     <t>Mux</t>
@@ -292,13 +292,22 @@
     <t>RF SMA PCB connector</t>
   </si>
   <si>
-    <t>507-1800-1-ND</t>
-  </si>
-  <si>
-    <t>350mA fuse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B5819WS-TPMSCT-ND </t>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>Blue LED</t>
+  </si>
+  <si>
+    <t>Yellow LED</t>
+  </si>
+  <si>
+    <t>732-4966-1-ND</t>
+  </si>
+  <si>
+    <t>732-4971-1-ND</t>
+  </si>
+  <si>
+    <t>732-4981-1-ND</t>
   </si>
 </sst>
 </file>
@@ -658,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,12 +742,15 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
+      <c r="E2" s="8">
+        <v>2</v>
+      </c>
       <c r="F2" s="2">
         <v>4.12</v>
       </c>
       <c r="G2" s="2">
         <f>E2*F2</f>
-        <v>0</v>
+        <v>8.24</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>27</v>
@@ -750,14 +762,14 @@
         <v>1</v>
       </c>
       <c r="L2" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M2" s="2">
         <v>2.84</v>
       </c>
       <c r="N2" s="2">
         <f>L2*M2</f>
-        <v>5.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -770,12 +782,15 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
       <c r="F3" s="2">
         <v>5.95</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" ref="G3:G10" si="0">E3*F3</f>
-        <v>0</v>
+        <v>5.95</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>29</v>
@@ -786,15 +801,15 @@
       <c r="K3" s="1">
         <v>1</v>
       </c>
-      <c r="L3" s="1">
-        <v>2</v>
+      <c r="L3" s="8">
+        <v>0</v>
       </c>
       <c r="M3" s="2">
         <v>2.77</v>
       </c>
       <c r="N3" s="2">
         <f t="shared" ref="N3:N16" si="1">L3*M3</f>
-        <v>5.54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -807,12 +822,15 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
+      <c r="E4" s="8">
+        <v>2</v>
+      </c>
       <c r="F4" s="2">
         <v>1.23</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.46</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>22</v>
@@ -823,15 +841,15 @@
       <c r="K4" s="1">
         <v>1</v>
       </c>
-      <c r="L4" s="1">
-        <v>2</v>
+      <c r="L4" s="8">
+        <v>0</v>
       </c>
       <c r="M4" s="2">
         <v>0.55000000000000004</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -844,12 +862,15 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
+      <c r="E5" s="8">
+        <v>2</v>
+      </c>
       <c r="F5" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>25</v>
@@ -860,15 +881,15 @@
       <c r="K5" s="1">
         <v>1</v>
       </c>
-      <c r="L5" s="1">
-        <v>2</v>
+      <c r="L5" s="8">
+        <v>0</v>
       </c>
       <c r="M5" s="2">
         <v>0.65</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" si="1"/>
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -881,12 +902,15 @@
       <c r="C6" s="1">
         <v>2</v>
       </c>
+      <c r="E6" s="8">
+        <v>10</v>
+      </c>
       <c r="F6" s="2">
-        <v>0.67</v>
+        <v>0.437</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.37</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>50</v>
@@ -897,15 +921,15 @@
       <c r="K6" s="1">
         <v>1</v>
       </c>
-      <c r="L6" s="1">
-        <v>2</v>
+      <c r="L6" s="8">
+        <v>0</v>
       </c>
       <c r="M6" s="2">
         <v>0.16</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="1"/>
-        <v>0.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -918,12 +942,15 @@
       <c r="C7" s="1">
         <v>5</v>
       </c>
+      <c r="E7" s="8">
+        <v>10</v>
+      </c>
       <c r="F7" s="2">
         <v>0.15</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>51</v>
@@ -934,15 +961,15 @@
       <c r="K7" s="1">
         <v>1</v>
       </c>
-      <c r="L7" s="1">
-        <v>2</v>
+      <c r="L7" s="8">
+        <v>0</v>
       </c>
       <c r="M7" s="2">
         <v>0.28000000000000003</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="1"/>
-        <v>0.56000000000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -955,12 +982,15 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
+      <c r="E8" s="8">
+        <v>10</v>
+      </c>
       <c r="F8" s="2">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>52</v>
@@ -971,15 +1001,15 @@
       <c r="K8" s="1">
         <v>1</v>
       </c>
-      <c r="L8" s="1">
-        <v>2</v>
+      <c r="L8" s="8">
+        <v>0</v>
       </c>
       <c r="M8" s="2">
         <v>0.2</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -992,12 +1022,15 @@
       <c r="C9" s="1">
         <v>6</v>
       </c>
+      <c r="E9" s="8">
+        <v>10</v>
+      </c>
       <c r="F9" s="2">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>53</v>
@@ -1008,15 +1041,15 @@
       <c r="K9" s="1">
         <v>1</v>
       </c>
-      <c r="L9" s="1">
-        <v>2</v>
+      <c r="L9" s="8">
+        <v>0</v>
       </c>
       <c r="M9" s="2">
         <v>0.25</v>
       </c>
       <c r="N9" s="2">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1029,18 +1062,24 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
+      <c r="E10" s="8">
+        <v>10</v>
+      </c>
       <c r="F10" s="2">
         <v>1.9E-2</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K10" s="1">
         <v>2</v>
+      </c>
+      <c r="L10" s="8">
+        <v>0</v>
       </c>
       <c r="N10" s="2">
         <f t="shared" si="1"/>
@@ -1060,6 +1099,9 @@
       <c r="C11" s="1">
         <v>2</v>
       </c>
+      <c r="E11" s="8">
+        <v>10</v>
+      </c>
       <c r="I11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1069,15 +1111,15 @@
       <c r="K11" s="1">
         <v>1</v>
       </c>
-      <c r="L11" s="1">
-        <v>1</v>
+      <c r="L11" s="8">
+        <v>0</v>
       </c>
       <c r="M11" s="2">
         <v>6.81</v>
       </c>
       <c r="N11" s="2">
         <f t="shared" si="1"/>
-        <v>6.81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -1090,6 +1132,12 @@
       <c r="C12" s="1">
         <v>2</v>
       </c>
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="I12" s="1" t="s">
         <v>34</v>
       </c>
@@ -1099,15 +1147,15 @@
       <c r="K12" s="1">
         <v>1</v>
       </c>
-      <c r="L12" s="1">
-        <v>1</v>
+      <c r="L12" s="8">
+        <v>0</v>
       </c>
       <c r="M12" s="2">
         <v>14.95</v>
       </c>
       <c r="N12" s="2">
         <f t="shared" si="1"/>
-        <v>14.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -1120,12 +1168,15 @@
       <c r="C13" s="1">
         <v>1</v>
       </c>
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
       <c r="F13" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="G13" s="2">
         <f>E13*F13</f>
-        <v>0</v>
+        <v>0.21999999999999997</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>35</v>
@@ -1136,15 +1187,15 @@
       <c r="K13" s="1">
         <v>1</v>
       </c>
-      <c r="L13" s="1">
-        <v>2</v>
+      <c r="L13" s="8">
+        <v>0</v>
       </c>
       <c r="M13" s="2">
         <v>12.5</v>
       </c>
       <c r="N13" s="2">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -1157,12 +1208,15 @@
       <c r="C14" s="3">
         <v>5</v>
       </c>
+      <c r="E14" s="1">
+        <v>10</v>
+      </c>
       <c r="F14" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G14" s="2">
         <f>E14*F14</f>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>59</v>
@@ -1173,15 +1227,15 @@
       <c r="K14" s="1">
         <v>1</v>
       </c>
-      <c r="L14" s="1">
-        <v>1</v>
+      <c r="L14" s="8">
+        <v>0</v>
       </c>
       <c r="M14" s="5">
         <v>2.95</v>
       </c>
       <c r="N14" s="2">
         <f t="shared" si="1"/>
-        <v>2.95</v>
+        <v>0</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>63</v>
@@ -1197,12 +1251,15 @@
       <c r="C15" s="1">
         <v>3</v>
       </c>
+      <c r="E15" s="1">
+        <v>10</v>
+      </c>
       <c r="F15" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G15" s="2">
         <f>E15*F15</f>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>60</v>
@@ -1213,15 +1270,15 @@
       <c r="K15" s="1">
         <v>1</v>
       </c>
-      <c r="L15" s="1">
-        <v>1</v>
+      <c r="L15" s="8">
+        <v>0</v>
       </c>
       <c r="M15" s="2">
         <v>1.25</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>64</v>
@@ -1237,6 +1294,16 @@
       <c r="C16" s="1">
         <v>1</v>
       </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="G16" s="2">
+        <f>E16*F16</f>
+        <v>2.9699999999999998</v>
+      </c>
       <c r="I16" s="1" t="s">
         <v>62</v>
       </c>
@@ -1246,15 +1313,15 @@
       <c r="K16" s="1">
         <v>1</v>
       </c>
-      <c r="L16" s="1">
-        <v>1</v>
+      <c r="L16" s="8">
+        <v>0</v>
       </c>
       <c r="M16" s="2">
         <v>3.05</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="1"/>
-        <v>3.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1267,12 +1334,15 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
+      <c r="E17" s="1">
+        <v>2</v>
+      </c>
       <c r="F17" s="2">
         <v>0.52</v>
       </c>
       <c r="G17" s="2">
         <f>E17*F17</f>
-        <v>0</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1286,112 +1356,186 @@
         <v>1</v>
       </c>
       <c r="D18" s="6"/>
+      <c r="E18" s="1">
+        <v>3</v>
+      </c>
       <c r="F18" s="2">
         <v>2.33</v>
       </c>
       <c r="G18" s="2">
         <f>E18*F18</f>
-        <v>0</v>
+        <v>6.99</v>
       </c>
       <c r="N18" s="2">
         <f>SUM(N2:N16)</f>
-        <v>69.41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="8">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G19" s="2">
+        <f>E19*F19</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="8">
+        <v>3</v>
       </c>
       <c r="F20" s="2">
-        <v>2.17</v>
+        <v>0.16</v>
       </c>
       <c r="G20" s="2">
-        <f>E20*F20</f>
-        <v>0</v>
-      </c>
+        <f t="shared" ref="G20:G21" si="2">E20*F20</f>
+        <v>0.48</v>
+      </c>
+      <c r="M20" s="2"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>72</v>
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>93</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="2"/>
+        <v>0.42000000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
+        <v>87</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2</v>
       </c>
       <c r="F22" s="2">
-        <v>0.2</v>
+        <v>2.17</v>
+      </c>
+      <c r="G22" s="2">
+        <f>E22*F22</f>
+        <v>4.34</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3</v>
       </c>
       <c r="F23" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="G23" s="2">
+        <f>E23*F23</f>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G28" s="2">
-        <f>SUM(G2:G27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>67</v>
+      <c r="G24" s="2">
+        <f>E24*F24</f>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G27" s="2">
+        <f>SUM(G2:G24)</f>
+        <v>42.29</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>79</v>
+        <v>66</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1402,9 +1546,9 @@
     <hyperlink ref="J12" r:id="rId3" xr:uid="{F8FCF166-57E3-4B3F-A665-042561BF6934}"/>
     <hyperlink ref="J15" r:id="rId4" xr:uid="{FBC8E941-7B24-4FAF-ACEB-DD0438F6BDD9}"/>
     <hyperlink ref="J16" r:id="rId5" xr:uid="{47868E09-3EC4-42BC-8E64-F5105C27F835}"/>
-    <hyperlink ref="B36" r:id="rId6" xr:uid="{5C805838-9D7A-4A69-B716-8DBFF1B315E3}"/>
-    <hyperlink ref="B35" r:id="rId7" xr:uid="{2DE54676-3B1A-4A9B-8385-E44AE31DB6F7}"/>
-    <hyperlink ref="B34" r:id="rId8" xr:uid="{8C8CAB8B-5DD6-4EB4-AD24-EE91835A4ED0}"/>
+    <hyperlink ref="B37" r:id="rId6" xr:uid="{5C805838-9D7A-4A69-B716-8DBFF1B315E3}"/>
+    <hyperlink ref="B36" r:id="rId7" xr:uid="{2DE54676-3B1A-4A9B-8385-E44AE31DB6F7}"/>
+    <hyperlink ref="B35" r:id="rId8" xr:uid="{8C8CAB8B-5DD6-4EB4-AD24-EE91835A4ED0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>

</xml_diff>

<commit_message>
added crystal to BOM
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.3-bom.xlsx
+++ b/sedani/estop/estop-1.3-bom.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D780EC-453C-45FD-9ABE-C2BC38B7E288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ACEB27-C542-4312-8AC3-7CADF40C075A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -308,6 +308,12 @@
   </si>
   <si>
     <t>732-4981-1-ND</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>SER4070CT-ND</t>
   </si>
 </sst>
 </file>
@@ -667,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1175,7 +1181,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="G13" s="2">
-        <f>E13*F13</f>
+        <f t="shared" ref="G13:G20" si="2">E13*F13</f>
         <v>0.21999999999999997</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1215,7 +1221,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G14" s="2">
-        <f>E14*F14</f>
+        <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -1258,7 +1264,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G15" s="2">
-        <f>E15*F15</f>
+        <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -1301,7 +1307,7 @@
         <v>0.99</v>
       </c>
       <c r="G16" s="2">
-        <f>E16*F16</f>
+        <f t="shared" si="2"/>
         <v>2.9699999999999998</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -1341,201 +1347,217 @@
         <v>0.52</v>
       </c>
       <c r="G17" s="2">
-        <f>E17*F17</f>
+        <f t="shared" si="2"/>
         <v>1.04</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="1">
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="1">
         <v>3</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="2">
         <v>2.33</v>
       </c>
-      <c r="G18" s="2">
-        <f>E18*F18</f>
+      <c r="G19" s="2">
+        <f t="shared" si="2"/>
         <v>6.99</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N19" s="2">
         <f>SUM(N2:N16)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="8">
-        <v>2</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8">
-        <v>5</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G19" s="2">
-        <f>E19*F19</f>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="8">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="8">
-        <v>1</v>
-      </c>
-      <c r="E20" s="8">
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="E21" s="8">
         <v>3</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F21" s="2">
         <v>0.16</v>
       </c>
-      <c r="G20" s="2">
-        <f t="shared" ref="G20:G21" si="2">E20*F20</f>
+      <c r="G21" s="2">
+        <f t="shared" ref="G21:G22" si="3">E21*F21</f>
         <v>0.48</v>
       </c>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1">
-        <v>3</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G21" s="2">
-        <f t="shared" si="2"/>
-        <v>0.42000000000000004</v>
-      </c>
+      <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" s="2">
-        <v>2.17</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G22" s="2">
-        <f>E22*F22</f>
-        <v>4.34</v>
+        <f t="shared" si="3"/>
+        <v>0.42000000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23">
+        <v>87</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" s="2">
-        <v>0.16</v>
+        <v>2.17</v>
       </c>
       <c r="G23" s="2">
         <f>E23*F23</f>
-        <v>0.48</v>
+        <v>4.34</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="1">
+        <v>70</v>
+      </c>
+      <c r="C24">
         <v>1</v>
       </c>
       <c r="E24" s="1">
         <v>3</v>
       </c>
       <c r="F24" s="2">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="G24" s="2">
         <f>E24*F24</f>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="G25" s="2">
+        <f>E25*F25</f>
         <v>0.39</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G27" s="2">
-        <f>SUM(G2:G24)</f>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G28" s="2">
+        <f>SUM(G2:G25)</f>
         <v>42.29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>79</v>
+        <v>66</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1546,9 +1568,9 @@
     <hyperlink ref="J12" r:id="rId3" xr:uid="{F8FCF166-57E3-4B3F-A665-042561BF6934}"/>
     <hyperlink ref="J15" r:id="rId4" xr:uid="{FBC8E941-7B24-4FAF-ACEB-DD0438F6BDD9}"/>
     <hyperlink ref="J16" r:id="rId5" xr:uid="{47868E09-3EC4-42BC-8E64-F5105C27F835}"/>
-    <hyperlink ref="B37" r:id="rId6" xr:uid="{5C805838-9D7A-4A69-B716-8DBFF1B315E3}"/>
-    <hyperlink ref="B36" r:id="rId7" xr:uid="{2DE54676-3B1A-4A9B-8385-E44AE31DB6F7}"/>
-    <hyperlink ref="B35" r:id="rId8" xr:uid="{8C8CAB8B-5DD6-4EB4-AD24-EE91835A4ED0}"/>
+    <hyperlink ref="B38" r:id="rId6" xr:uid="{5C805838-9D7A-4A69-B716-8DBFF1B315E3}"/>
+    <hyperlink ref="B37" r:id="rId7" xr:uid="{2DE54676-3B1A-4A9B-8385-E44AE31DB6F7}"/>
+    <hyperlink ref="B36" r:id="rId8" xr:uid="{8C8CAB8B-5DD6-4EB4-AD24-EE91835A4ED0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>

</xml_diff>

<commit_message>
updated level shifter part
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.3-bom.xlsx
+++ b/sedani/estop/estop-1.3-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ACEB27-C542-4312-8AC3-7CADF40C075A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA872EFA-E4D0-475B-8177-BC490AEC5AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,9 +262,6 @@
     <t>MC74HC157ADGOS-ND</t>
   </si>
   <si>
-    <t>296-1135-1-ND</t>
-  </si>
-  <si>
     <t>APX823-31W5GDICT-ND</t>
   </si>
   <si>
@@ -314,6 +311,9 @@
   </si>
   <si>
     <t>SER4070CT-ND</t>
+  </si>
+  <si>
+    <t>296-20631-1-ND</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,10 +1097,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1130,10 +1130,10 @@
     </row>
     <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1292,10 +1292,10 @@
     </row>
     <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -1335,7 +1335,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -1353,10 +1353,10 @@
     </row>
     <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" t="s">
         <v>94</v>
-      </c>
-      <c r="B18" t="s">
-        <v>95</v>
       </c>
       <c r="C18" s="8">
         <v>1</v>
@@ -1372,7 +1372,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -1395,10 +1395,10 @@
     </row>
     <row r="20" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="8">
         <v>2</v>
@@ -1419,10 +1419,10 @@
     </row>
     <row r="21" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="8">
         <v>1</v>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>18</v>
@@ -1542,7 +1542,7 @@
         <v>74</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
making sure right part number in sheet
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.3-bom.xlsx
+++ b/sedani/estop/estop-1.3-bom.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA872EFA-E4D0-475B-8177-BC490AEC5AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DA6D35-1CAB-4BE0-85F1-EF2F41CB6579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -676,7 +676,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>